<commit_message>
Improve temperature-page code and GUI
Add conversion from Celsius to Fahrenheit into the nextion GUI and made according changes to the arduino code. Correct EEPROM addresses
</commit_message>
<xml_diff>
--- a/Bill of Material (BOM).xlsx
+++ b/Bill of Material (BOM).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOCmaniac\Documents\GitHub\Universal-3D-Printer-Smart-Enclosure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DC97E5-80EE-4A50-886A-CFBAD7F23AE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89345187-B083-4489-911A-D1C0FC243422}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>Part</t>
   </si>
@@ -90,9 +90,6 @@
     <t>1500mm</t>
   </si>
   <si>
-    <t>970mm</t>
-  </si>
-  <si>
     <t>Aluminum profile black 30x30 B-type slot 9</t>
   </si>
   <si>
@@ -145,6 +142,39 @@
   </si>
   <si>
     <t>Nextion enhanced 5inch dispplay (NX8048K050)</t>
+  </si>
+  <si>
+    <t>Panels/Floor</t>
+  </si>
+  <si>
+    <t>MDF 4mm</t>
+  </si>
+  <si>
+    <t>MDF 8mm</t>
+  </si>
+  <si>
+    <t>515x515mm</t>
+  </si>
+  <si>
+    <t>MDF 18mm</t>
+  </si>
+  <si>
+    <t>490x490mm</t>
+  </si>
+  <si>
+    <t>Spool compartment floor and printer compartment ceiling panels</t>
+  </si>
+  <si>
+    <t>Printer compartment floor</t>
+  </si>
+  <si>
+    <t>515x517mm</t>
+  </si>
+  <si>
+    <t>Side panels - 2 panels fits inside 1 60cm by 120cm panel (48in by 24in)</t>
+  </si>
+  <si>
+    <t>967mm</t>
   </si>
 </sst>
 </file>
@@ -214,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -223,9 +253,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -258,6 +285,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -543,308 +576,350 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.7109375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2</v>
+      </c>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="12">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="12">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="12">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="12">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="12">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="12">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="12">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="17">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="17">
+        <v>2</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="17">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="13">
+      <c r="B17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="12">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="12">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="13">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="13">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="13">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="13">
-        <v>16</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="13">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="13">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="13">
-        <v>12</v>
-      </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="13">
-        <v>3</v>
-      </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="13">
+      <c r="E19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="15">
         <v>1</v>
       </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="13">
-        <v>24</v>
-      </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="13">
+      <c r="E20" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="12">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="13">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="13">
-        <v>2</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="16">
-        <v>1</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="13">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="10"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="10"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="10"/>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="9"/>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -856,29 +931,38 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E27" s="2"/>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="2"/>
+    </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-      <c r="D30" s="18"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D31" s="18"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D32" s="18"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="18"/>
-    </row>
-    <row r="34" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="19"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="19"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="19"/>
+    </row>
+    <row r="37" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E2:E3"/>
-    <mergeCell ref="D30:D33"/>
+    <mergeCell ref="D33:D36"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>